<commit_message>
Added notes on excel formulas
</commit_message>
<xml_diff>
--- a/Display/RGB Display Spreadsheet.xlsx
+++ b/Display/RGB Display Spreadsheet.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RGB Color Map" sheetId="1" r:id="rId1"/>
+    <sheet name="Excel Function  Examples" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="21">
   <si>
     <t>R</t>
   </si>
@@ -48,6 +49,45 @@
   </si>
   <si>
     <t>6 Bytes</t>
+  </si>
+  <si>
+    <t>Cell A1 contains the name of another cell: A3</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>Cell A2 contains the formula: =INDIRECT(A1) which causes the value of the cell to be what is in A3</t>
+  </si>
+  <si>
+    <t>Cell A3 contains: Hi</t>
+  </si>
+  <si>
+    <t>Cell A5 contains the formula: =ADDRESS(1,1)</t>
+  </si>
+  <si>
+    <t>Cell A6 contains the formula: =ADDRESS(1,1,1) // Absolute</t>
+  </si>
+  <si>
+    <t>Cell A7 contains the formula: =ADDRESS(1,1,2) // Absolute Row, Relative Column</t>
+  </si>
+  <si>
+    <t>Cell A8 contains the formula: =ADDRESS(1,1,2) // Relative Row, Absolute Column</t>
+  </si>
+  <si>
+    <t>Cell A9 contains the formula: =ADDRESS(1,1,4) // Relative</t>
+  </si>
+  <si>
+    <t>Cell A11 contains the formula: =CELL("address", A1)</t>
+  </si>
+  <si>
+    <t>=CELL("row",INDIRECT(CELL("address",A1)))</t>
+  </si>
+  <si>
+    <t>=CELL("col",INDIRECT(CELL("address",A1)))</t>
   </si>
 </sst>
 </file>
@@ -154,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -167,6 +207,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -182,7 +223,28 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -196,28 +258,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -499,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1260,22 +1301,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AG17">
-    <cfRule type="cellIs" dxfId="1" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"B"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"RG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"RB"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"GB"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -1285,4 +1326,152 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="89" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f ca="1">INDIRECT(A1)</f>
+        <v>Hi</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>ADDRESS(1,1)</f>
+        <v>$A$1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>ADDRESS(1,1,1)</f>
+        <v>$A$1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>ADDRESS(1,1,2)</f>
+        <v>A$1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>ADDRESS(1,1,3)</f>
+        <v>$A1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>ADDRESS(1,1,4)</f>
+        <v>A1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f ca="1">CELL("address", A1)</f>
+        <v>$A$1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" ref="A12:A14" ca="1" si="0">CELL("address", A2)</f>
+        <v>$A$2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>$A$3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>$A$4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f ca="1">CELL("row",INDIRECT(CELL("address",A1)))</f>
+        <v>1</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f ca="1">CELL("col",INDIRECT(CELL("address",A1)))</f>
+        <v>1</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="str">
+        <f ca="1">TEXT(A11,"")</f>
+        <v>$A$1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>